<commit_message>
Adds creation of steel markets
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-smr-atr-biogas.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-smr-atr-biogas.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2181" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2182" uniqueCount="208">
   <si>
     <t>Database</t>
   </si>
@@ -1048,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M475"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A232" workbookViewId="0">
-      <selection activeCell="I252" sqref="I252"/>
+    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
+      <selection activeCell="A253" sqref="A253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5708,6 +5708,9 @@
       <c r="A254" t="s">
         <v>12</v>
       </c>
+      <c r="B254" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="255" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A255" t="s">

</xml_diff>

<commit_message>
Produces region-specific fuel pathways (work in progress)
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-smr-atr-biogas.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-smr-atr-biogas.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual" iterate="1" iterateCount="15" iterateDelta="0.05"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1006,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M407"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="B138" sqref="B138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3174,7 +3174,7 @@
         <v>35</v>
       </c>
       <c r="B109">
-        <v>2.9996721816189444E-3</v>
+        <v>6.84</v>
       </c>
       <c r="C109" t="s">
         <v>27</v>
@@ -3200,7 +3200,7 @@
         <v>41</v>
       </c>
       <c r="B110">
-        <v>0.38041197561668283</v>
+        <v>2.9996721816189444E-3</v>
       </c>
       <c r="C110" t="s">
         <v>27</v>
@@ -3226,7 +3226,7 @@
         <v>49</v>
       </c>
       <c r="B111">
-        <v>5.3487471618165237E-10</v>
+        <v>0.38041197561668283</v>
       </c>
       <c r="C111" t="s">
         <v>27</v>
@@ -3246,7 +3246,7 @@
         <v>56</v>
       </c>
       <c r="B112">
-        <v>5.3272799999999989E-4</v>
+        <v>5.3487471618165237E-10</v>
       </c>
       <c r="C112" t="s">
         <v>122</v>
@@ -3269,7 +3269,7 @@
         <v>59</v>
       </c>
       <c r="B113">
-        <v>3.6000000000000001E-5</v>
+        <v>5.3272799999999989E-4</v>
       </c>
       <c r="C113" t="s">
         <v>122</v>
@@ -3292,7 +3292,7 @@
         <v>62</v>
       </c>
       <c r="B114">
-        <v>3.6239999999999997E-4</v>
+        <v>3.6000000000000001E-5</v>
       </c>
       <c r="C114" t="s">
         <v>122</v>
@@ -3315,7 +3315,7 @@
         <v>64</v>
       </c>
       <c r="B115">
-        <v>2.54628E-9</v>
+        <v>3.6239999999999997E-4</v>
       </c>
       <c r="C115" t="s">
         <v>122</v>
@@ -3338,7 +3338,7 @@
         <v>68</v>
       </c>
       <c r="B116">
-        <v>2.796E-5</v>
+        <v>2.54628E-9</v>
       </c>
       <c r="C116" t="s">
         <v>122</v>
@@ -3361,7 +3361,7 @@
         <v>70</v>
       </c>
       <c r="B117">
-        <v>1.668E-5</v>
+        <v>2.796E-5</v>
       </c>
       <c r="C117" t="s">
         <v>122</v>
@@ -3384,7 +3384,7 @@
         <v>72</v>
       </c>
       <c r="B118">
-        <v>2.0292014459767036E-4</v>
+        <v>1.668E-5</v>
       </c>
       <c r="C118" t="s">
         <v>122</v>
@@ -3407,7 +3407,7 @@
         <v>188</v>
       </c>
       <c r="B119">
-        <v>3.1235999999999997E-4</v>
+        <v>2.0292014459767036E-4</v>
       </c>
       <c r="C119" t="s">
         <v>122</v>
@@ -3430,7 +3430,7 @@
         <v>74</v>
       </c>
       <c r="B120">
-        <v>4.8000000000000001E-5</v>
+        <v>3.1235999999999997E-4</v>
       </c>
       <c r="C120" t="s">
         <v>122</v>
@@ -3453,7 +3453,7 @@
         <v>76</v>
       </c>
       <c r="B121">
-        <v>1.1591999999999998E-5</v>
+        <v>4.8000000000000001E-5</v>
       </c>
       <c r="C121" t="s">
         <v>122</v>
@@ -3476,7 +3476,7 @@
         <v>78</v>
       </c>
       <c r="B122">
-        <v>7.5385438054847107</v>
+        <v>1.1591999999999998E-5</v>
       </c>
       <c r="C122" t="s">
         <v>122</v>
@@ -3499,7 +3499,7 @@
         <v>80</v>
       </c>
       <c r="B123">
-        <v>8.8290154606725723E-4</v>
+        <v>7.5390157563601576</v>
       </c>
       <c r="C123" t="s">
         <v>122</v>
@@ -3522,7 +3522,7 @@
         <v>83</v>
       </c>
       <c r="B124">
-        <v>3.7140000000000003E-4</v>
+        <v>8.8290154606725723E-4</v>
       </c>
       <c r="C124" t="s">
         <v>122</v>
@@ -3545,7 +3545,7 @@
         <v>85</v>
       </c>
       <c r="B125">
-        <v>-0.67249589978061108</v>
+        <v>3.7140000000000003E-4</v>
       </c>
       <c r="C125" t="s">
         <v>122</v>
@@ -3568,7 +3568,7 @@
         <v>87</v>
       </c>
       <c r="B126">
-        <v>5.1637924671186237</v>
+        <v>-0.61975263847726747</v>
       </c>
       <c r="C126" t="s">
         <v>122</v>
@@ -3591,10 +3591,10 @@
         <v>54</v>
       </c>
       <c r="B127">
-        <v>4.3031603892655201E-2</v>
+        <v>3.9205289542065938</v>
       </c>
       <c r="C127" t="s">
-        <v>53</v>
+        <v>122</v>
       </c>
       <c r="D127" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Update SMR and ATR H2 inventories.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-smr-atr-biogas.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-smr-atr-biogas.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10507"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9F1AD0-15CB-B846-BD0D-7F2DF734B48E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A50DEB4-2B3C-D940-A8F2-03E1C0502281}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="27040" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1025,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M411"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A138" sqref="A138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1709,7 +1709,8 @@
         <v>53</v>
       </c>
       <c r="B35">
-        <v>5.0788017117687465</v>
+        <f>(120*B4)/36</f>
+        <v>4.2790277666149539</v>
       </c>
       <c r="C35" t="s">
         <v>52</v>
@@ -2738,7 +2739,8 @@
         <v>53</v>
       </c>
       <c r="B85">
-        <v>5.1817707576649816</v>
+        <f>(120*B55)/36</f>
+        <v>4.36578197193682</v>
       </c>
       <c r="C85" t="s">
         <v>52</v>
@@ -3634,7 +3636,8 @@
         <v>53</v>
       </c>
       <c r="B130">
-        <v>3.9205289542065938</v>
+        <f>(120*B103)/36</f>
+        <v>4.3506347760410122</v>
       </c>
       <c r="C130" t="s">
         <v>119</v>
@@ -4231,7 +4234,8 @@
         <v>53</v>
       </c>
       <c r="B162">
-        <v>5.1638404545185992</v>
+        <f>(120*B133)/36</f>
+        <v>4.350675206723011</v>
       </c>
       <c r="C162" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
Zero out the co-production of electricity in SMR and ATR datasets.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-smr-atr-biogas.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-smr-atr-biogas.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C672D02C-DEDF-6D44-9B66-9BA916152F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDF4989C-F45F-C949-8047-012E82950B64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1260" yWindow="760" windowWidth="27040" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13,7 +13,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$M$244</definedName>
   </definedNames>
-  <calcPr calcId="191029" iterate="1" iterateDelta="0.01" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -821,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView tabSelected="1" topLeftCell="A198" workbookViewId="0">
+      <selection activeCell="B162" sqref="B162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2883,7 +2883,7 @@
         <v>82</v>
       </c>
       <c r="B100">
-        <v>-1.3016123468668273</v>
+        <v>0</v>
       </c>
       <c r="C100" t="s">
         <v>52</v>
@@ -3411,7 +3411,7 @@
         <v>82</v>
       </c>
       <c r="B129">
-        <v>-0.61975263847726747</v>
+        <v>0</v>
       </c>
       <c r="C129" t="s">
         <v>86</v>
@@ -4009,7 +4009,7 @@
         <v>82</v>
       </c>
       <c r="B161">
-        <v>-0.15423412693187019</v>
+        <v>0</v>
       </c>
       <c r="C161" t="s">
         <v>86</v>

</xml_diff>

<commit_message>
Fix factory input in ATR/SMR H2 datasets
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-smr-atr-biogas.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-smr-atr-biogas.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10119"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7BA3336-1697-D54A-A6BF-77DC32C57925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C661C9C6-69C8-6A4B-9D76-C929B5BF9132}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2660" yWindow="7100" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1081" uniqueCount="149">
   <si>
     <t>Database</t>
   </si>
@@ -479,6 +479,9 @@
   </si>
   <si>
     <t>negative</t>
+  </si>
+  <si>
+    <t>Original ecoinvent value.</t>
   </si>
 </sst>
 </file>
@@ -540,7 +543,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -549,6 +552,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -831,8 +835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L212"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="L213" sqref="L213"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1589,8 +1593,8 @@
       <c r="A38" t="s">
         <v>51</v>
       </c>
-      <c r="B38">
-        <v>5.3483393537845907E-10</v>
+      <c r="B38" s="6">
+        <v>2.6180197338995299E-11</v>
       </c>
       <c r="C38" t="s">
         <v>52</v>
@@ -1606,6 +1610,9 @@
       </c>
       <c r="H38" t="s">
         <v>53</v>
+      </c>
+      <c r="I38" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
@@ -2668,8 +2675,8 @@
       <c r="A90" t="s">
         <v>51</v>
       </c>
-      <c r="B90">
-        <v>5.3483199147628007E-10</v>
+      <c r="B90" s="6">
+        <v>2.6180197338995299E-11</v>
       </c>
       <c r="C90" t="s">
         <v>52</v>
@@ -2685,6 +2692,9 @@
       </c>
       <c r="H90" t="s">
         <v>53</v>
+      </c>
+      <c r="I90" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.2">
@@ -3244,8 +3254,8 @@
       <c r="A121" t="s">
         <v>51</v>
       </c>
-      <c r="B121">
-        <v>5.3487471618165237E-10</v>
+      <c r="B121" s="6">
+        <v>2.6180197338995299E-11</v>
       </c>
       <c r="C121" t="s">
         <v>86</v>
@@ -3261,6 +3271,9 @@
       </c>
       <c r="H121" t="s">
         <v>53</v>
+      </c>
+      <c r="I121" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.2">
@@ -3866,8 +3879,8 @@
       <c r="A154" t="s">
         <v>51</v>
       </c>
-      <c r="B154">
-        <v>5.3487623280160849E-10</v>
+      <c r="B154" s="6">
+        <v>2.6180197338995299E-11</v>
       </c>
       <c r="C154" t="s">
         <v>86</v>
@@ -3883,6 +3896,9 @@
       </c>
       <c r="H154" t="s">
         <v>53</v>
+      </c>
+      <c r="I154" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fix SMR Biogas LCIs.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-smr-atr-biogas.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-smr-atr-biogas.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10315"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F33AE566-7D16-47B5-8A92-62049B2149D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBCC2375-D3A7-5E49-811A-602A5B87056F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$J$208</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$P$208</definedName>
     <definedName name="m3_per_gallon">[1]Inputs!$E$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="151">
   <si>
     <t>Database</t>
   </si>
@@ -433,6 +433,69 @@
   <si>
     <t>Source: Hydrogen production from natural gas and biomethane with carbon capture and storage – A techno-environmental analysis. 2020. Antonini et al. https://doi.org/10.1039/D0SE00222D. This inventory represents the case "ATR BM, HT+LT+MDEA, 98 average" from that publication with the following changes: (a) Compression of H2 from 26 bar to 200 bar is omitted, which changes the power balance for excess power to grid from -17.39 MWe to -6.2 MWe (see Figure 2 in the publication). External power requirement is calculated to be 0.69kWh/kgH2.  (b) The water balance is changed to account for actual water consumption in the process or evaporated water only. 
 Biomethane: 0.722 kg/m3 at standard condition @ 15°C, 1.0325 bar. LHV by mass: 45.4 MJ/kg. LHV by volume at standard condition: 36.1 MJ/Nm3.</t>
+  </si>
+  <si>
+    <t>negative</t>
+  </si>
+  <si>
+    <t>US EPA 1998, high uncertainty reported qulitatively therein</t>
+  </si>
+  <si>
+    <t>rough estimate, high uncertainty</t>
+  </si>
+  <si>
+    <t>90% capture rate</t>
+  </si>
+  <si>
+    <t>measurement, single CC power plant</t>
+  </si>
+  <si>
+    <t>estimate from range of values from different references</t>
+  </si>
+  <si>
+    <t>heating value and efficiency</t>
+  </si>
+  <si>
+    <t>basic uncertainty for heavy metal; trace element in natural gas</t>
+  </si>
+  <si>
+    <t>range of values from different references</t>
+  </si>
+  <si>
+    <t>P. Jansohn (50 ppm in the flue gas; SCR -85% minus 1-3ppm due to capture)</t>
+  </si>
+  <si>
+    <t>composition of natural gas</t>
+  </si>
+  <si>
+    <t>NOx retained, by selective catalytic reduction</t>
+  </si>
+  <si>
+    <t>P. Jansohn (50 ppm in the flue gas; SCR -85)</t>
+  </si>
+  <si>
+    <t>gas power plant, combined cycle, 400MW electrical</t>
+  </si>
+  <si>
+    <t>n_plant = 1/(lifetime*annual fuel input)</t>
+  </si>
+  <si>
+    <t>hydrochloric acid, without water, in 30% solution state</t>
+  </si>
+  <si>
+    <t>basic uncertainty:1.05;(4,na,3,1,1,na)</t>
+  </si>
+  <si>
+    <t>sodium hydroxide, without water, in 50% solution state</t>
+  </si>
+  <si>
+    <t>water, decarbonised</t>
+  </si>
+  <si>
+    <t>biogas from biowaste</t>
+  </si>
+  <si>
+    <t>residue from cooling tower</t>
   </si>
 </sst>
 </file>
@@ -440,12 +503,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.0E+00"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.0E+00"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -495,20 +565,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -857,19 +926,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P208"/>
+  <dimension ref="A1:L208"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
+      <selection activeCell="E185" sqref="E185"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="67.7109375" customWidth="1"/>
+    <col min="1" max="1" width="67.6640625" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -877,7 +948,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -885,7 +956,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -893,7 +964,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -901,7 +972,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -909,7 +980,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -917,7 +988,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>103</v>
       </c>
@@ -925,49 +996,49 @@
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>120</v>
       </c>
@@ -989,14 +1060,8 @@
       <c r="H12" t="s">
         <v>119</v>
       </c>
-      <c r="K12" s="8"/>
-      <c r="L12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="8"/>
-      <c r="P12" s="8"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1021,14 +1086,8 @@
       <c r="H13" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="8"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1053,14 +1112,8 @@
       <c r="H14" t="s">
         <v>26</v>
       </c>
-      <c r="K14" s="8"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="P14" s="8"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1085,14 +1138,8 @@
       <c r="H15" t="s">
         <v>26</v>
       </c>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1117,14 +1164,8 @@
       <c r="H16" t="s">
         <v>26</v>
       </c>
-      <c r="K16" s="8"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1149,14 +1190,8 @@
       <c r="H17" t="s">
         <v>26</v>
       </c>
-      <c r="K17" s="8"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="8"/>
-      <c r="P17" s="8"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>107</v>
       </c>
@@ -1181,14 +1216,8 @@
       <c r="H18" t="s">
         <v>26</v>
       </c>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1213,14 +1242,8 @@
       <c r="H19" t="s">
         <v>26</v>
       </c>
-      <c r="K19" s="8"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1245,14 +1268,8 @@
       <c r="H20" t="s">
         <v>26</v>
       </c>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -1277,14 +1294,8 @@
       <c r="H21" t="s">
         <v>26</v>
       </c>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -1309,14 +1320,8 @@
       <c r="H22" t="s">
         <v>26</v>
       </c>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -1341,14 +1346,8 @@
       <c r="H23" t="s">
         <v>26</v>
       </c>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -1373,14 +1372,8 @@
       <c r="H24" t="s">
         <v>26</v>
       </c>
-      <c r="K24" s="8"/>
-      <c r="L24" s="8"/>
-      <c r="M24" s="8"/>
-      <c r="N24" s="8"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -1405,14 +1398,8 @@
       <c r="H25" t="s">
         <v>26</v>
       </c>
-      <c r="K25" s="8"/>
-      <c r="L25" s="8"/>
-      <c r="M25" s="8"/>
-      <c r="N25" s="8"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -1437,14 +1424,8 @@
       <c r="H26" t="s">
         <v>26</v>
       </c>
-      <c r="K26" s="8"/>
-      <c r="L26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="N26" s="8"/>
-      <c r="O26" s="8"/>
-      <c r="P26" s="8"/>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -1469,14 +1450,8 @@
       <c r="H27" t="s">
         <v>26</v>
       </c>
-      <c r="K27" s="8"/>
-      <c r="L27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="8"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="8"/>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -1501,14 +1476,8 @@
       <c r="H28" t="s">
         <v>26</v>
       </c>
-      <c r="K28" s="8"/>
-      <c r="L28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="8"/>
-      <c r="O28" s="8"/>
-      <c r="P28" s="8"/>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -1534,7 +1503,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -1560,7 +1529,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -1586,7 +1555,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -1612,7 +1581,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>114</v>
       </c>
@@ -1632,7 +1601,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>114</v>
       </c>
@@ -1655,7 +1624,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>108</v>
       </c>
@@ -1678,7 +1647,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>111</v>
       </c>
@@ -1701,7 +1670,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>50</v>
       </c>
@@ -1727,7 +1696,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>53</v>
       </c>
@@ -1750,7 +1719,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>56</v>
       </c>
@@ -1773,7 +1742,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>58</v>
       </c>
@@ -1796,7 +1765,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>60</v>
       </c>
@@ -1819,7 +1788,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>62</v>
       </c>
@@ -1842,7 +1811,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>64</v>
       </c>
@@ -1865,7 +1834,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>66</v>
       </c>
@@ -1888,7 +1857,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>105</v>
       </c>
@@ -1911,7 +1880,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>68</v>
       </c>
@@ -1934,7 +1903,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>70</v>
       </c>
@@ -1957,7 +1926,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>72</v>
       </c>
@@ -1980,7 +1949,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>74</v>
       </c>
@@ -2003,7 +1972,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>77</v>
       </c>
@@ -2026,7 +1995,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>79</v>
       </c>
@@ -2049,11 +2018,11 @@
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>81</v>
       </c>
-      <c r="B52" s="10">
+      <c r="B52" s="8">
         <v>8.9637775580545271E-3</v>
       </c>
       <c r="C52" t="s">
@@ -2072,7 +2041,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>1</v>
       </c>
@@ -2080,7 +2049,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>2</v>
       </c>
@@ -2088,7 +2057,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>5</v>
       </c>
@@ -2096,7 +2065,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>10</v>
       </c>
@@ -2104,7 +2073,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>8</v>
       </c>
@@ -2112,7 +2081,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>103</v>
       </c>
@@ -2120,46 +2089,46 @@
         <v>104</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>10</v>
       </c>
-      <c r="B61" s="7" t="s">
+      <c r="B61" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E63" t="s">
+      <c r="E63" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F63" t="s">
+      <c r="F63" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G63" t="s">
+      <c r="G63" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H63" t="s">
+      <c r="H63" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>118</v>
       </c>
@@ -2182,11 +2151,11 @@
         <v>119</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>24</v>
       </c>
-      <c r="B65" s="9">
+      <c r="B65" s="7">
         <v>3.1712942535739586E-8</v>
       </c>
       <c r="C65" t="s">
@@ -2208,11 +2177,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>29</v>
       </c>
-      <c r="B66" s="9">
+      <c r="B66" s="7">
         <v>4.7569413803609367E-6</v>
       </c>
       <c r="C66" t="s">
@@ -2234,11 +2203,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>30</v>
       </c>
-      <c r="B67" s="9">
+      <c r="B67" s="7">
         <v>1.268547829628838E-5</v>
       </c>
       <c r="C67" t="s">
@@ -2260,11 +2229,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>31</v>
       </c>
-      <c r="B68" s="9">
+      <c r="B68" s="7">
         <v>3.1712942535739584E-10</v>
       </c>
       <c r="C68" t="s">
@@ -2286,11 +2255,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>32</v>
       </c>
-      <c r="B69" s="9">
+      <c r="B69" s="7">
         <v>2.2199662339002805E-5</v>
       </c>
       <c r="C69" t="s">
@@ -2312,11 +2281,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>107</v>
       </c>
-      <c r="B70" s="9">
+      <c r="B70" s="7">
         <v>8.9153165218958783</v>
       </c>
       <c r="C70" t="s">
@@ -2338,11 +2307,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>33</v>
       </c>
-      <c r="B71" s="9">
+      <c r="B71" s="7">
         <v>6.6598384453023306E-5</v>
       </c>
       <c r="C71" t="s">
@@ -2364,11 +2333,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>34</v>
       </c>
-      <c r="B72" s="9">
+      <c r="B72" s="7">
         <v>3.1712942535739587E-6</v>
       </c>
       <c r="C72" t="s">
@@ -2390,11 +2359,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>35</v>
       </c>
-      <c r="B73" s="9">
+      <c r="B73" s="7">
         <v>3.1712942535739587E-6</v>
       </c>
       <c r="C73" t="s">
@@ -2416,11 +2385,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>36</v>
       </c>
-      <c r="B74" s="9">
+      <c r="B74" s="7">
         <v>9.5141840427144231E-10</v>
       </c>
       <c r="C74" t="s">
@@ -2442,11 +2411,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>37</v>
       </c>
-      <c r="B75" s="9">
+      <c r="B75" s="7">
         <v>6.3428897891404663E-5</v>
       </c>
       <c r="C75" t="s">
@@ -2468,11 +2437,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>38</v>
       </c>
-      <c r="B76" s="9">
+      <c r="B76" s="7">
         <v>5.6767553036139577E-4</v>
       </c>
       <c r="C76" t="s">
@@ -2494,11 +2463,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>39</v>
       </c>
-      <c r="B77" s="9">
+      <c r="B77" s="7">
         <v>3.1712942535739582E-7</v>
       </c>
       <c r="C77" t="s">
@@ -2520,11 +2489,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>40</v>
       </c>
-      <c r="B78" s="9">
+      <c r="B78" s="7">
         <v>6.3428897891404652E-6</v>
       </c>
       <c r="C78" t="s">
@@ -2546,11 +2515,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>41</v>
       </c>
-      <c r="B79" s="9">
+      <c r="B79" s="7">
         <v>3.805794129882789E-5</v>
       </c>
       <c r="C79" t="s">
@@ -2572,11 +2541,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>42</v>
       </c>
-      <c r="B80" s="9">
+      <c r="B80" s="7">
         <v>6.3428897891404652E-6</v>
       </c>
       <c r="C80" t="s">
@@ -2598,11 +2567,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>43</v>
       </c>
-      <c r="B81" s="9">
+      <c r="B81" s="7">
         <v>6.3428897891404654E-7</v>
       </c>
       <c r="C81" t="s">
@@ -2624,11 +2593,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>44</v>
       </c>
-      <c r="B82" s="9">
+      <c r="B82" s="7">
         <v>1.7442720958641867E-5</v>
       </c>
       <c r="C82" t="s">
@@ -2650,11 +2619,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>45</v>
       </c>
-      <c r="B83" s="9">
+      <c r="B83" s="7">
         <v>6.3428897891404652E-6</v>
       </c>
       <c r="C83" t="s">
@@ -2676,11 +2645,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>46</v>
       </c>
-      <c r="B84" s="9">
+      <c r="B84" s="7">
         <v>0.38037452713377901</v>
       </c>
       <c r="C84" t="s">
@@ -2702,11 +2671,11 @@
         <v>26</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>114</v>
       </c>
-      <c r="B85" s="9">
+      <c r="B85" s="7">
         <v>0.37128651379599975</v>
       </c>
       <c r="C85" t="s">
@@ -2722,11 +2691,11 @@
         <v>28</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>114</v>
       </c>
-      <c r="B86" s="9">
+      <c r="B86" s="7">
         <v>9.0880133377792584E-3</v>
       </c>
       <c r="C86" t="s">
@@ -2745,11 +2714,11 @@
         <v>116</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>111</v>
       </c>
-      <c r="B87" s="9">
+      <c r="B87" s="7">
         <v>4.8020529894434176</v>
       </c>
       <c r="C87" t="s">
@@ -2768,11 +2737,11 @@
         <v>112</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>50</v>
       </c>
-      <c r="B88" s="9">
+      <c r="B88" s="7">
         <v>5.3483199147628007E-10</v>
       </c>
       <c r="C88" t="s">
@@ -2794,11 +2763,11 @@
         <v>123</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>53</v>
       </c>
-      <c r="B89" s="9">
+      <c r="B89" s="7">
         <v>5.3272799999999989E-4</v>
       </c>
       <c r="C89" t="s">
@@ -2817,11 +2786,11 @@
         <v>55</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>56</v>
       </c>
-      <c r="B90" s="9">
+      <c r="B90" s="7">
         <v>3.6000000000000001E-5</v>
       </c>
       <c r="C90" t="s">
@@ -2840,11 +2809,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>58</v>
       </c>
-      <c r="B91" s="9">
+      <c r="B91" s="7">
         <v>3.6239999999999997E-4</v>
       </c>
       <c r="C91" t="s">
@@ -2863,11 +2832,11 @@
         <v>59</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>62</v>
       </c>
-      <c r="B92" s="9">
+      <c r="B92" s="7">
         <v>2.54628E-9</v>
       </c>
       <c r="C92" t="s">
@@ -2886,11 +2855,11 @@
         <v>63</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>64</v>
       </c>
-      <c r="B93" s="9">
+      <c r="B93" s="7">
         <v>2.796E-5</v>
       </c>
       <c r="C93" t="s">
@@ -2909,11 +2878,11 @@
         <v>65</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>66</v>
       </c>
-      <c r="B94" s="9">
+      <c r="B94" s="7">
         <v>1.668E-5</v>
       </c>
       <c r="C94" t="s">
@@ -2932,11 +2901,11 @@
         <v>67</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>105</v>
       </c>
-      <c r="B95" s="9">
+      <c r="B95" s="7">
         <v>2.0292014459767036E-4</v>
       </c>
       <c r="C95" t="s">
@@ -2955,11 +2924,11 @@
         <v>106</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>68</v>
       </c>
-      <c r="B96" s="9">
+      <c r="B96" s="7">
         <v>3.1235999999999997E-4</v>
       </c>
       <c r="C96" t="s">
@@ -2978,11 +2947,11 @@
         <v>69</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>70</v>
       </c>
-      <c r="B97" s="9">
+      <c r="B97" s="7">
         <v>4.8000000000000001E-5</v>
       </c>
       <c r="C97" t="s">
@@ -3001,11 +2970,11 @@
         <v>71</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>72</v>
       </c>
-      <c r="B98" s="9">
+      <c r="B98" s="7">
         <v>1.1591999999999998E-5</v>
       </c>
       <c r="C98" t="s">
@@ -3024,11 +2993,11 @@
         <v>73</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>74</v>
       </c>
-      <c r="B99" s="9">
+      <c r="B99" s="7">
         <v>4.430822860844585</v>
       </c>
       <c r="C99" t="s">
@@ -3047,11 +3016,11 @@
         <v>76</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>77</v>
       </c>
-      <c r="B100" s="9">
+      <c r="B100" s="7">
         <v>8.8290154606725723E-4</v>
       </c>
       <c r="C100" t="s">
@@ -3070,11 +3039,11 @@
         <v>78</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>79</v>
       </c>
-      <c r="B101" s="9">
+      <c r="B101" s="7">
         <v>3.7140000000000003E-4</v>
       </c>
       <c r="C101" t="s">
@@ -3093,7 +3062,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>81</v>
       </c>
@@ -3119,7 +3088,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
         <v>1</v>
       </c>
@@ -3127,7 +3096,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>2</v>
       </c>
@@ -3135,7 +3104,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>5</v>
       </c>
@@ -3143,7 +3112,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>8</v>
       </c>
@@ -3151,7 +3120,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>103</v>
       </c>
@@ -3159,46 +3128,46 @@
         <v>104</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>10</v>
       </c>
-      <c r="B109" s="7" t="s">
+      <c r="B109" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A111" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B111" t="s">
+      <c r="B111" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C111" t="s">
+      <c r="C111" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D111" t="s">
+      <c r="D111" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E111" t="s">
+      <c r="E111" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F111" t="s">
+      <c r="F111" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G111" t="s">
+      <c r="G111" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H111" t="s">
+      <c r="H111" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>121</v>
       </c>
@@ -3221,7 +3190,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>107</v>
       </c>
@@ -3247,7 +3216,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>38</v>
       </c>
@@ -3273,7 +3242,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>46</v>
       </c>
@@ -3293,7 +3262,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>114</v>
       </c>
@@ -3313,7 +3282,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>114</v>
       </c>
@@ -3336,7 +3305,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>50</v>
       </c>
@@ -3362,7 +3331,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>53</v>
       </c>
@@ -3385,7 +3354,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>56</v>
       </c>
@@ -3408,7 +3377,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>58</v>
       </c>
@@ -3431,7 +3400,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>62</v>
       </c>
@@ -3454,7 +3423,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>64</v>
       </c>
@@ -3477,7 +3446,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>66</v>
       </c>
@@ -3500,7 +3469,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>105</v>
       </c>
@@ -3523,7 +3492,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>68</v>
       </c>
@@ -3546,7 +3515,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>70</v>
       </c>
@@ -3569,7 +3538,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>72</v>
       </c>
@@ -3592,7 +3561,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>74</v>
       </c>
@@ -3615,7 +3584,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>77</v>
       </c>
@@ -3638,7 +3607,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>79</v>
       </c>
@@ -3661,7 +3630,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>81</v>
       </c>
@@ -3687,7 +3656,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>111</v>
       </c>
@@ -3710,7 +3679,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="135" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A135" s="2" t="s">
         <v>1</v>
       </c>
@@ -3718,7 +3687,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>2</v>
       </c>
@@ -3726,7 +3695,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>5</v>
       </c>
@@ -3734,7 +3703,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>8</v>
       </c>
@@ -3742,7 +3711,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>103</v>
       </c>
@@ -3750,46 +3719,46 @@
         <v>104</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>10</v>
       </c>
-      <c r="B140" s="7" t="s">
+      <c r="B140" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="141" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A142" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B142" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C142" t="s">
+      <c r="C142" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D142" t="s">
+      <c r="D142" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E142" t="s">
+      <c r="E142" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F142" t="s">
+      <c r="F142" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G142" t="s">
+      <c r="G142" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H142" t="s">
+      <c r="H142" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>122</v>
       </c>
@@ -3812,7 +3781,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>107</v>
       </c>
@@ -3838,7 +3807,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>38</v>
       </c>
@@ -3864,7 +3833,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>46</v>
       </c>
@@ -3884,7 +3853,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>114</v>
       </c>
@@ -3904,7 +3873,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>114</v>
       </c>
@@ -3927,7 +3896,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>108</v>
       </c>
@@ -3950,7 +3919,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>50</v>
       </c>
@@ -3976,7 +3945,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>53</v>
       </c>
@@ -3999,7 +3968,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>56</v>
       </c>
@@ -4022,7 +3991,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>58</v>
       </c>
@@ -4045,7 +4014,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>60</v>
       </c>
@@ -4068,7 +4037,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>62</v>
       </c>
@@ -4091,7 +4060,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>64</v>
       </c>
@@ -4114,7 +4083,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>66</v>
       </c>
@@ -4137,7 +4106,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>105</v>
       </c>
@@ -4160,7 +4129,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>68</v>
       </c>
@@ -4183,7 +4152,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>70</v>
       </c>
@@ -4206,7 +4175,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>72</v>
       </c>
@@ -4229,7 +4198,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>74</v>
       </c>
@@ -4252,7 +4221,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>77</v>
       </c>
@@ -4275,7 +4244,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>79</v>
       </c>
@@ -4298,7 +4267,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>81</v>
       </c>
@@ -4321,7 +4290,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>111</v>
       </c>
@@ -4344,7 +4313,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="168" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A168" s="2" t="s">
         <v>1</v>
       </c>
@@ -4352,7 +4321,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>2</v>
       </c>
@@ -4360,7 +4329,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>4</v>
       </c>
@@ -4368,7 +4337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="171" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>5</v>
       </c>
@@ -4376,7 +4345,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>6</v>
       </c>
@@ -4384,7 +4353,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>8</v>
       </c>
@@ -4392,12 +4361,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="174" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A174" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>12</v>
       </c>
@@ -4425,9 +4394,17 @@
       <c r="I175" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J175" s="1"/>
-    </row>
-    <row r="176" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="J175" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K175" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L175" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="176" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A176" s="3" t="s">
         <v>110</v>
       </c>
@@ -4446,8 +4423,14 @@
       <c r="F176" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J176" t="s">
+        <v>26</v>
+      </c>
+      <c r="K176" s="9" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>89</v>
       </c>
@@ -4472,8 +4455,11 @@
       <c r="I177">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K177" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>24</v>
       </c>
@@ -4498,8 +4484,11 @@
       <c r="I178">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K178" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>29</v>
       </c>
@@ -4524,8 +4513,11 @@
       <c r="I179">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K179" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>30</v>
       </c>
@@ -4550,8 +4542,11 @@
       <c r="I180">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K180" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>31</v>
       </c>
@@ -4576,8 +4571,11 @@
       <c r="I181">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K181" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>32</v>
       </c>
@@ -4602,8 +4600,11 @@
       <c r="I182">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K182" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>107</v>
       </c>
@@ -4628,8 +4629,11 @@
       <c r="I183">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K183" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>91</v>
       </c>
@@ -4654,8 +4658,11 @@
       <c r="I184">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K184" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>34</v>
       </c>
@@ -4680,8 +4687,11 @@
       <c r="I185">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K185" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>92</v>
       </c>
@@ -4706,8 +4716,11 @@
       <c r="I186">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K186" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>93</v>
       </c>
@@ -4732,8 +4745,11 @@
       <c r="I187">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K187" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>35</v>
       </c>
@@ -4758,8 +4774,11 @@
       <c r="I188">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K188" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>94</v>
       </c>
@@ -4784,8 +4803,11 @@
       <c r="I189">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K189" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>95</v>
       </c>
@@ -4810,8 +4832,11 @@
       <c r="I190">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K190" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>36</v>
       </c>
@@ -4836,8 +4861,11 @@
       <c r="I191">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K191" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>84</v>
       </c>
@@ -4862,8 +4890,11 @@
       <c r="I192">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K192" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="193" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>38</v>
       </c>
@@ -4888,8 +4919,11 @@
       <c r="I193">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K193" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="194" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>39</v>
       </c>
@@ -4914,8 +4948,11 @@
       <c r="I194">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K194" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="195" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>40</v>
       </c>
@@ -4940,8 +4977,11 @@
       <c r="I195">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K195" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="196" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>41</v>
       </c>
@@ -4966,8 +5006,11 @@
       <c r="I196">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K196" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="197" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>42</v>
       </c>
@@ -4992,8 +5035,11 @@
       <c r="I197">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K197" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="198" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>43</v>
       </c>
@@ -5018,8 +5064,11 @@
       <c r="I198">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K198" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="199" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>44</v>
       </c>
@@ -5044,8 +5093,11 @@
       <c r="I199">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K199" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="200" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>45</v>
       </c>
@@ -5070,8 +5122,11 @@
       <c r="I200">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K200" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="201" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>109</v>
       </c>
@@ -5096,8 +5151,11 @@
       <c r="I201">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K201" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="202" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>100</v>
       </c>
@@ -5122,8 +5180,14 @@
       <c r="I202">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J202" t="s">
+        <v>141</v>
+      </c>
+      <c r="K202" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="203" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>96</v>
       </c>
@@ -5148,8 +5212,14 @@
       <c r="I203">
         <v>0.57209088006881903</v>
       </c>
-    </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J203" t="s">
+        <v>143</v>
+      </c>
+      <c r="K203" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="204" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>97</v>
       </c>
@@ -5174,8 +5244,14 @@
       <c r="I204">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J204" t="s">
+        <v>145</v>
+      </c>
+      <c r="K204" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="205" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>98</v>
       </c>
@@ -5200,8 +5276,14 @@
       <c r="I205">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J205" t="s">
+        <v>147</v>
+      </c>
+      <c r="K205" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="206" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>102</v>
       </c>
@@ -5226,8 +5308,14 @@
       <c r="I206">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J206" t="s">
+        <v>148</v>
+      </c>
+      <c r="K206" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="207" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>111</v>
       </c>
@@ -5252,8 +5340,14 @@
       <c r="I207">
         <v>0.25816898211842121</v>
       </c>
-    </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J207" t="s">
+        <v>112</v>
+      </c>
+      <c r="K207" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="208" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>99</v>
       </c>
@@ -5278,8 +5372,18 @@
       <c r="I208">
         <v>0.25816898211842121</v>
       </c>
+      <c r="J208" t="s">
+        <v>150</v>
+      </c>
+      <c r="K208" t="s">
+        <v>132</v>
+      </c>
+      <c r="L208" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:P208" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>